<commit_message>
Update MSc Stats Data 2021-23 Batch BARC.xlsx
</commit_message>
<xml_diff>
--- a/2023/BARC/MSc Stats Data 2021-23 Batch BARC.xlsx
+++ b/2023/BARC/MSc Stats Data 2021-23 Batch BARC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Student CV\cv\2023\BARC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\cv\2023\BARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31092EF-1287-4DC6-AA25-2622C1E07217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1207244C-EC85-4554-81B3-14AC37581A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B6D54597-654D-47FE-930E-933B921A294B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6D54597-654D-47FE-930E-933B921A294B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -335,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -348,18 +348,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -679,29 +673,29 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="115.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="38" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="63.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>71</v>
       </c>
       <c r="B1" t="s">
@@ -747,7 +741,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -757,13 +751,13 @@
       <c r="C2">
         <v>9922546958</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <v>2017</v>
       </c>
       <c r="G2">
@@ -772,32 +766,32 @@
       <c r="H2">
         <v>2020</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>79</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <f>455/6</f>
         <v>75.833333333333329</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <f>453/6</f>
         <v>75.5</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <f>406/6</f>
         <v>67.666666666666671</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <f t="shared" ref="M2:M16" si="0">AVERAGE(J2:L2)</f>
         <v>73</v>
       </c>
-      <c r="O2" s="14" t="str">
+      <c r="O2" s="10" t="str">
         <f t="shared" ref="O2:O16" si="1">HYPERLINK(_xlfn.CONCAT("https://kbcnmustats.github.io/cv/2023/BARC/",A2,".pdf"))</f>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Gore Prachi Ganpat.pdf</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
@@ -833,17 +827,17 @@
       <c r="L3">
         <v>78.66</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <f t="shared" si="0"/>
         <v>72.33</v>
       </c>
-      <c r="O3" s="14" t="str">
+      <c r="O3" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Patil Vaishnavi Sharad.pdf</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
@@ -852,13 +846,13 @@
       <c r="C4">
         <v>9960323237</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4">
         <v>2018</v>
       </c>
       <c r="G4">
@@ -879,20 +873,20 @@
       <c r="L4">
         <v>69.66</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <f t="shared" si="0"/>
         <v>71.44</v>
       </c>
       <c r="N4" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="14" t="str">
+      <c r="O4" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Salunke Chetan Rajaram.pdf</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
@@ -928,20 +922,20 @@
       <c r="L5">
         <v>70.83</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <f t="shared" si="0"/>
         <v>69.553333333333327</v>
       </c>
       <c r="N5" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="14" t="str">
+      <c r="O5" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Fulpagare Pradip Shantaram.pdf</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6" t="s">
@@ -977,17 +971,17 @@
       <c r="L6">
         <v>73.33</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <f t="shared" si="0"/>
         <v>66.606666666666669</v>
       </c>
-      <c r="O6" s="14" t="str">
+      <c r="O6" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Mahajan Kanchan Jayant.pdf</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
@@ -996,44 +990,44 @@
       <c r="C7">
         <v>9370860580</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7">
         <v>2018</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>89</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7">
         <v>2021</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="5">
         <v>0.89600000000000002</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7">
         <v>65</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7">
         <v>64</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7">
         <v>69</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="O7" s="14" t="str">
+      <c r="O7" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Bari Mayuri Rajesh.pdf</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" t="s">
@@ -1069,17 +1063,17 @@
       <c r="L8">
         <v>68.33</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <f t="shared" si="0"/>
         <v>65.663333333333341</v>
       </c>
-      <c r="O8" s="14" t="str">
+      <c r="O8" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Puranik Yashashri Madhav.pdf</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
@@ -1112,20 +1106,20 @@
       <c r="L9">
         <v>65.16</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <f t="shared" si="0"/>
         <v>62.886666666666663</v>
       </c>
       <c r="N9" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="14" t="str">
+      <c r="O9" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Patil Diksha Dilip.pdf</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
@@ -1161,16 +1155,16 @@
       <c r="L10">
         <v>64.5</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <f t="shared" si="0"/>
         <v>62.833333333333336</v>
       </c>
-      <c r="O10" s="14" t="str">
+      <c r="O10" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Patil Hemant Prakash.pdf</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1198,32 +1192,32 @@
       <c r="I11">
         <v>70.03</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <f>417/6</f>
         <v>69.5</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <f>358/6</f>
         <v>59.666666666666664</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <f>335/6</f>
         <v>55.833333333333336</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <f t="shared" si="0"/>
         <v>61.666666666666664</v>
       </c>
       <c r="N11" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="14" t="str">
+      <c r="O11" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Patil Nikita Sharad.pdf</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>47</v>
       </c>
       <c r="B12" t="s">
@@ -1259,17 +1253,17 @@
       <c r="L12">
         <v>69.16</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <f t="shared" si="0"/>
         <v>61.386666666666663</v>
       </c>
-      <c r="O12" s="14" t="str">
+      <c r="O12" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Patil Sopan Raman.pdf</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
@@ -1305,17 +1299,17 @@
       <c r="L13">
         <v>61.35</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <f t="shared" si="0"/>
         <v>61.336666666666666</v>
       </c>
-      <c r="O13" s="14" t="str">
+      <c r="O13" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Patil Vaishnavi Pradip.pdf</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -1324,44 +1318,44 @@
       <c r="C14">
         <v>9373255242</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14">
         <v>2018</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14">
         <v>63.54</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14">
         <v>2021</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" t="s">
         <v>66</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14">
         <v>61.67</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14">
         <v>56.169999999999995</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14">
         <v>62.17</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <f t="shared" si="0"/>
         <v>60.00333333333333</v>
       </c>
-      <c r="O14" s="14" t="str">
+      <c r="O14" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Yeola Bhanuja Bharat.pdf</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
       <c r="B15" t="s">
@@ -1370,13 +1364,13 @@
       <c r="C15">
         <v>7350141762</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <v>2018</v>
       </c>
       <c r="G15">
@@ -1397,16 +1391,16 @@
       <c r="L15">
         <v>63.16</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <f t="shared" si="0"/>
         <v>59.54999999999999</v>
       </c>
-      <c r="O15" s="14" t="str">
+      <c r="O15" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Ghogare Sachin Nanasaheb.pdf</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1443,11 +1437,11 @@
       <c r="L16" s="4">
         <v>52.33</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
-      <c r="O16" s="14" t="str">
+      <c r="O16" s="10" t="str">
         <f t="shared" si="1"/>
         <v>https://kbcnmustats.github.io/cv/2023/BARC/Chaudhari Jayesh Suresh.pdf</v>
       </c>

</xml_diff>